<commit_message>
added backend code to allow users to sign up
</commit_message>
<xml_diff>
--- a/SKAZ_DB_maps.xlsx
+++ b/SKAZ_DB_maps.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/06f113a1f573cf4f/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/06f113a1f573cf4f/Documents/GitHub/AA1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="577" documentId="8_{04B64F91-40C6-411C-8FC6-A81B4327CA50}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{EBA82360-8DA0-4702-AED1-E230037F7D43}"/>
+  <xr:revisionPtr revIDLastSave="581" documentId="8_{04B64F91-40C6-411C-8FC6-A81B4327CA50}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{7E52665C-63C9-4DF1-AD98-F676A0BE1297}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{A18279E6-D1D1-42AF-9792-7BCFB476BF08}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A18279E6-D1D1-42AF-9792-7BCFB476BF08}"/>
   </bookViews>
   <sheets>
     <sheet name="master_stories" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="182">
   <si>
     <t>String</t>
   </si>
@@ -444,9 +444,6 @@
   </si>
   <si>
     <t>password_salt</t>
-  </si>
-  <si>
-    <t>company_user</t>
   </si>
   <si>
     <t>is_consumer</t>
@@ -686,12 +683,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -700,7 +712,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -749,14 +761,26 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1090,15 +1114,15 @@
   <sheetData>
     <row r="1" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -1278,7 +1302,7 @@
     </row>
     <row r="19" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>4</v>
@@ -1327,8 +1351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB1ABD2-7E29-4031-87F9-5C48D3FF4383}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1340,169 +1364,186 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>4</v>
-      </c>
+      <c r="B3" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="24"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" s="24"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="24"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="24"/>
+    </row>
+    <row r="7" spans="1:3" ht="93.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="24"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="24"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="C10" s="24"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="C11" s="24"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="C12" s="24"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="24"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14" s="24" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="C14" s="24"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="B15" s="24" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="C15" s="24"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="B16" s="24" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="93.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="C16" s="24"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="24"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="B18" s="24" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+      <c r="C18" s="24"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="C19" s="24"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>147</v>
-      </c>
+      <c r="B20" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="C20" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1516,15 +1557,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F83736C7-2185-4E5D-AF56-E8CDCB0D75AE}">
   <dimension ref="A2:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -1547,18 +1591,18 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
+        <v>176</v>
+      </c>
+      <c r="F3" t="s">
         <v>177</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>178</v>
-      </c>
-      <c r="G3" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -1566,7 +1610,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -1594,11 +1638,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="A1" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -1613,7 +1657,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>4</v>
@@ -1621,7 +1665,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>0</v>
@@ -1629,7 +1673,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>2</v>
@@ -1637,7 +1681,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>3</v>
@@ -1662,11 +1706,11 @@
   <sheetFormatPr defaultColWidth="28.140625" defaultRowHeight="51" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
     </row>
     <row r="2" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -1758,13 +1802,13 @@
     </row>
     <row r="10" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>45</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.3">
@@ -1799,11 +1843,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
     </row>
     <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -1857,7 +1901,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -1879,7 +1923,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -1901,7 +1945,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -1912,7 +1956,7 @@
         <v>3</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -1923,7 +1967,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1934,7 +1978,7 @@
         <v>17</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
@@ -1945,7 +1989,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
@@ -1965,7 +2009,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1976,7 +2020,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1987,7 +2031,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1998,7 +2042,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -2009,7 +2053,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2034,11 +2078,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -2059,7 +2103,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2070,7 +2114,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2081,7 +2125,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -2092,7 +2136,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -2103,7 +2147,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -2114,7 +2158,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2125,17 +2169,17 @@
         <v>4</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="18" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2147,7 +2191,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
@@ -2158,7 +2202,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -2169,7 +2213,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2180,12 +2224,12 @@
         <v>45</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>4</v>
@@ -2205,7 +2249,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:B9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2214,11 +2258,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
     </row>
     <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -2269,7 +2313,7 @@
         <v>121</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>26</v>
@@ -2280,7 +2324,7 @@
         <v>120</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>28</v>
@@ -2291,7 +2335,7 @@
         <v>125</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>29</v>
@@ -2302,7 +2346,7 @@
         <v>117</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>31</v>
@@ -2338,11 +2382,11 @@
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
     </row>
     <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">

</xml_diff>